<commit_message>
minor bugfixes and annotations
</commit_message>
<xml_diff>
--- a/proj_aged/core/aged/lab/DataSafeOnes/05_good_AgedStock_only_two_brands.xlsx
+++ b/proj_aged/core/aged/lab/DataSafeOnes/05_good_AgedStock_only_two_brands.xlsx
@@ -251,14 +251,16 @@
   </sheetPr>
   <dimension ref="A1:J233"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H21" activeCellId="0" sqref="H21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.3828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.16"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
partial functional tests for available stock page (filters and search bar). Small bugfix
</commit_message>
<xml_diff>
--- a/proj_aged/core/aged/lab/DataSafeOnes/05_good_AgedStock_only_two_brands.xlsx
+++ b/proj_aged/core/aged/lab/DataSafeOnes/05_good_AgedStock_only_two_brands.xlsx
@@ -124,7 +124,7 @@
     <t xml:space="preserve">CHO-010-672</t>
   </si>
   <si>
-    <t xml:space="preserve">NUTS</t>
+    <t xml:space="preserve">NUTS.</t>
   </si>
   <si>
     <t xml:space="preserve">HK BAKING STICKS 5KG/UC 4UC/BOX</t>
@@ -252,10 +252,10 @@
   <dimension ref="A1:J233"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.40625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.76"/>

</xml_diff>